<commit_message>
Added counters summary output
You can now export the list of erorrs per attribute as a summarised spreadsheet.
</commit_message>
<xml_diff>
--- a/examples/bristol bus stops/profile.xlsx
+++ b/examples/bristol bus stops/profile.xlsx
@@ -500,7 +500,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -510,14 +510,14 @@
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
-        <v>17410</v>
+        <v>18904</v>
       </c>
       <c r="S2" t="n">
         <v>1600</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>['1', '10000001', '1000053203', '1000053204', '1000053205', '1000053206', '1000053207', '1000053208', '1000053209', '1000053210', '1000053211', '1000053212', '1000053214', '1000053216', '1000053217', '1000053218', '1000053219', '1000053220', '1000053221', '1000053222', '1000053223', '1000053227', '1000053228', '1000053229', '1000053230', '1000053231', '1000053276', '1000053287', '1000053288', '1000053305', '1000053310', '1000053311', '1000053312', '100053233', '100053234', '100053236', '100053239', '100053240', '100053241', '100053247', '100053248', '100053249', '100053250', '100053252', '100053254', '100053255', '100053256', '100053257', '100053258', '100053259', '100053260', '100053261', '100053262', '100053263', '100053264', '100053265', '100053266', '100053267', '100053274', '100053275', '100053277', '100053278', '100053279', '100053280', '100053281', '100053283', '100053291', '100053293', '100053294', '100053295', '100053296', '100053297', '100053298', '100053299', '100053300', '100053301', '100053303', '100053304', '100053306', '100053309', '100053313', '100053315', '100053316', '100053317', '100053318', '100053319', '100053320', '100053321', '100053324', '100053325', '100053328', '100053329', '100053330', '100053331', '100053332', '100053333', '100053334', '100053335', '100053337', '100053338', '100053339', '100053340', '100053343', '100053344', '100053345', '100053346', '100BAC30684', '100BAC30685', '100BAC30742', '100BAC30743', '100BAC30946', '100BAZ02458', '100BAZ02459', '100BRA01797', '100BRA01798', '100BRA01799', '100BRA01800', '100BRA10006', '100BRA10007', '100BRA10008', '100BRA10009', '100BRA10010', '100BRA10011', '100BRA10012', '100BRA10013', '100BRA10014', '100BRA10015', '100BRA10016', '100BRA10021', '100BRA10022', '100BRA10023', '100BRA10024', '100BRA10025', '100BRA10026', '100BRA10027', '100BRA10029', '100BRA10030', '100BRA10031', '100BRA10032', '100BRA10033', '100BRA10034', '100BRA10035', '100BRA10036', '100BRA10037', '100BRA10038', '100BRA10039', '100BRA10040', '100BRA10041', '100BRA10042', '100BRA10047', '100BRA10048', '100BRA10049', '100BRA10050', '100BRA10051', '100BRA10052', '100BRA10053', '100BRA10054', '100BRA10055', '100BRA10056', '100BRA10057', '100BRA10059', '100BRA10062', '100BRA10064', '100BRA10065', '100BRA10066', '100BRA10067', '100BRA10068', '100BRA10069', '100BRA10070', '100BRA10071', '100BRA10072', '100BRA10073', '100BRA10074', '100BRA10075', '100BRA10076', '100BRA10077', '100BRA10078', '100BRA10079', '100BRA10080', '100BRA10081', '100BRA10082', '100BRA10083', '100BRA10084', '100BRA10086', '100BRA10087', '100BRA10088', '100BRA10089', '100BRA10090', '100BRA10091', '100BRA10092', '100BRA10093', '100BRA10094', '100BRA10095', '100BRA10096', '100BRA10097', '100BRA10098', '100BRA10099', '100BRA10100', '100BRA10101', '100BRA10102', '100BRA10103', '100BRA10104', '100BRA10105', '100BRA10106', '100BRA10107', '100BRA10108', '100BRA10109', '100BRA10110', '100BRA10111', '100BRA10112', '100BRA10113', '100BRA10114', '100BRA10115', '100BRA10116', '100BRA10117', '100BRA10119', '100BRA10120', '100BRA10121', '100BRA10122', '100BRA10123', '100BRA10124', '100BRA10125', '100BRA10126', '100BRA10127', '100BRA10128', '100BRA10129', '100BRA10130', '100BRA10131', '100BRA10132', '100BRA10133', '100BRA10134', '100BRA10135', '100BRA10136', '100BRA10137', '100BRA10138', '100BRA10139', '100BRA10140', '100BRA10143', '100BRA10144', '100BRA10145', '100BRA10146', '100BRA10147', '100BRA10148', '100BRA10149', '100BRA10150', '100BRA10151', '100BRA10152', '100BRA10153', '100BRA10154', '100BRA10155', '100BRA10156', '100BRA10157', '100BRA10158', '100BRA10159', '100BRA10160', '100BRA10161', '100BRA10162', '100BRA10163', '100BRA10164', '100BRA10165', '100BRA10166', '100BRA10167', '100BRA10168', '100BRA10169', '100BRA10170', '100BRA10171', '100BRA10172', '100BRA10173', '100BRA10174', '100BRA10175', '100BRA10176', '100BRA10177', '100BRA10178', '100BRA10179', '100BRA10180', '100BRA10181', '100BRA10182', '100BRA10183', '100BRA10184', '100BRA10187', '100BRA10188', '100BRA10189', '100BRA10190', '100BRA10191', '100BRA10192', '100BRA10193', '100BRA10195', '100BRA10196', '100BRA10197', '100BRA10198', '100BRA10199', '100BRA10200', '100BRA10201', '100BRA10202', '100BRA10203', '100BRA10204', '100BRA10205', '100BRA10206', '100BRA10207', '100BRA10208', '100BRA10209', '100BRA10210', '100BRA10211', '100BRA10212', '100BRA10213', '100BRA10214', '100BRA10215', '100BRA10216', '100BRA10217', '100BRA10218', '100BRA10219', '100BRA10220', '100BRA10221', '100BRA10225', '100BRA10229', '100BRA10230', '100BRA10231', '100BRA10233', '100BRA10235', '100BRA10236', '100BRA10237', '100BRA10238', '100BRA10239', '100BRA10240', '100BRA10241', '100BRA10242', '100BRA10243', '100BRA10244', '100BRA10245', '100BRA10246', '100BRA10247', '100BRA10248', '100BRA10249', '100BRA10250', '100BRA10251', '100BRA10252', '100BRA10253', '100BRA10254', '100BRA10255', '100BRA10256', '100BRA10257', '100BRA10258', '100BRA10259', '100BRA10260', '100BRA10261', '100BRA10262', '100BRA10263', '100BRA10264', '100BRA10265', '100BRA10266', '100BRA10267', '100BRA10269', '100BRA10270', '100BRA10272', '100BRA10273', '100BRA10274', '100BRA10275', '100BRA10276', '100BRA10277', '100BRA10278', '100BRA10279', '100BRA10280', '100BRA10281', '100BRA10282', '100BRA10283', '100BRA10284', '100BRA10285', '100BRA10286', '100BRA10287', '100BRA10288', '100BRA10289', '100BRA10290', '100BRA10291', '100BRA10292', '100BRA10293', '100BRA10294', '100BRA10295', '100BRA10296', '100BRA10297', '100BRA10298', '100BRA10299', '100BRA10300', '100BRA10301', '100BRA10302', '100BRA10303', '100BRA10304', '100BRA10305', '100BRA10306', '100BRA10308', '100BRA10309', '100BRA10311', '100BRA10312', '100BRA10313', '100BRA10315', '100BRA10316', '100BRA10317', '100BRA10318', '100BRA10319', '100BRA10320', '100BRA10321', '100BRA10323', '100BRA10324', '100BRA10325', '100BRA10326', '100BRA10327', '100BRA10328', '100BRA10329', '100BRA10330', '100BRA10331', '100BRA10332', '100BRA10333', '100BRA10334', '100BRA10335', '100BRA10336', '100BRA10337', '100BRA10339', '100BRA10340', '100BRA10342', '100BRA10343', '100BRA10344', '100BRA10352', '100BRA10353', '100BRA10354', '100BRA10355', '100BRA10356', '100BRA10357', '100BRA10358', '100BRA10359', '100BRA10360', '100BRA10361', '100BRA10362', '100BRA10363', '100BRA10364', '100BRA10365', '100BRA10366', '100BRA10367', '100BRA10368', '100BRA10369', '100BRA10370', '100BRA10371', '100BRA10372', '100BRA10373', '100BRA10374', '100BRA10375', '100BRA10376', '100BRA10377', '100BRA10378', '100BRA10381', '100BRA10382', '100BRA10383', '100BRA10384', '100BRA10385', '100BRA10386', '100BRA10392', '100BRA10393', '100BRA10394', '100BRA10395', '100BRA10396', '100BRA10397', '100BRA10398', '100BRA10399', '100BRA10400', '100BRA10401', '100BRA10403', '100BRA10404', '100BRA10405', '100BRA10406', '100BRA10407', '100BRA10408', '100BRA10409', '100BRA10410', '100BRA10411', '100BRA10412', '100BRA10413', '100BRA10414', '100BRA10415', '100BRA10417', '100BRA10418', '100BRA10419', '100BRA10421', '100BRA10423', '100BRA10425', '100BRA10426', '100BRA10427', '100BRA10428', '100BRA10429', '100BRA10430', '100BRA10431', '100BRA10432', '100BRA10433', '100BRA10434', '100BRA10435', '100BRA10436', '100BRA10437', '100BRA10438', '100BRA10439', '100BRA10440', '100BRA10441', '100BRA10442', '100BRA10443', '100BRA10444', '100BRA10445', '100BRA10446', '100BRA10447', '100BRA10448', '100BRA10449', '100BRA10450', '100BRA10451', '100BRA10452', '100BRA10453', '100BRA10454', '100BRA10455', '100BRA10456', '100BRA10457', '100BRA10458', '100BRA10459', '100BRA10460', '100BRA10461', '100BRA10464', '100BRA10465', '100BRA10466', '100BRA10467', '100BRA10468', '100BRA10469', '100BRA10470', '100BRA10471', '100BRA10472', '100BRA10473', '100BRA10474', '100BRA10475', '100BRA10476', '100BRA10477', '100BRA10478', '100BRA10479', '100BRA10480', '100BRA10481', '100BRA10482', '100BRA10483', '100BRA10484', '100BRA10485', '100BRA10486', '100BRA10487', '100BRA10488', '100BRA10489', '100BRA10490', '100BRA10491', '100BRA10492', '100BRA10493', '100BRA10494', '100BRA10495', '100BRA10496', '100BRA10497', '100BRA10498', '100BRA10499', '100BRA10500', '100BRA10501', '100BRA10502', '100BRA10503', '100BRA10504', '100BRA10505', '100BRA10506', '100BRA10507', '100BRA10508', '100BRA10509', '100BRA10510', '100BRA10511', '100BRA10512', '100BRA10513', '100BRA10514', '100BRA10515', '100BRA10516', '100BRA10521', '100BRA10522', '100BRA10523', '100BRA10524', '100BRA10525', '100BRA10527', '100BRA10528', '100BRA10529', '100BRA10530', '100BRA10531', '100BRA10532', '100BRA10533', '100BRA10534', '100BRA10535', '100BRA10536', '100BRA10537', '100BRA10538', '100BRA10539', '100BRA10540', '100BRA10543', '100BRA10544', '100BRA10545', '100BRA10546', '100BRA10547', '100BRA10548', '100BRA10549', '100BRA10550', '100BRA10551', '100BRA10553', '100BRA10554', '100BRA10555', '100BRA10556', '100BRA10557', '100BRA10558', '100BRA10559', '100BRA10560', '100BRA10561', '100BRA10562', '100BRA10563', '100BRA10564', '100BRA10565', '100BRA10566', '100BRA10567', '100BRA10570', '100BRA10571', '100BRA10572', '100BRA10574', '100BRA10575', '100BRA10576', '100BRA10577', '100BRA10578', '100BRA10579', '100BRA10580', '100BRA10583', '100BRA10584', '100BRA10585', '100BRA10586', '100BRA10587', '100BRA10588', '100BRA10589', '100BRA10590', '100BRA10591', '100BRA10592', '100BRA10593', '100BRA10594', '100BRA10595', '100BRA10596', '100BRA10598', '100BRA10599', '100BRA10600', '100BRA10601', '100BRA10602', '100BRA10603', '100BRA10604', '100BRA10605', '100BRA10606', '100BRA10607', '100BRA10608', '100BRA10609', '100BRA10614', '100BRA10616', '100BRA10617', '100BRA10618', '100BRA10619', '100BRA10620', '100BRA10621', '100BRA10622', '100BRA10623', '100BRA10624', '100BRA10625', '100BRA10626', '100BRA10627', '100BRA10628', '100BRA10629', '100BRA10630', '100BRA10631', '100BRA10632', '100BRA10633', '100BRA10634', '100BRA10635', '100BRA10636', '100BRA10637', '100BRA10638', '100BRA10639', '100BRA10640', '100BRA10641', '100BRA10642', '100BRA10643', '100BRA10644', '100BRA10645', '100BRA10647', '100BRA10648', '100BRA10649', '100BRA10650', '100BRA10651', '100BRA10652', '100BRA10653', '100BRA10654', '100BRA10655', '100BRA10656', '100BRA10657', '100BRA10658', '100BRA10659', '100BRA10660', '100BRA10661', '100BRA10662', '100BRA10663', '100BRA10665', '100BRA10666', '100BRA10667', '100BRA10668', '100BRA10669', '100BRA10673', '100BRA10674', '100BRA10675', '100BRA10676', '100BRA10677', '100BRA10678', '100BRA10679', '100BRA10680', '100BRA10681', '100BRA10682', '100BRA10683', '100BRA10684', '100BRA10685', '100BRA10686', '100BRA10687', '100BRA10691', '100BRA10692', '100BRA10693', '100BRA10696', '100BRA10697', '100BRA10698', '100BRA10699', '100BRA10700', '100BRA10701', '100BRA10702', '100BRA10703', '100BRA10704', '100BRA10706', '100BRA10707', '100BRA10708', '100BRA10709', '100BRA10710', '100BRA10711', '100BRA10712', '100BRA10713', '100BRA10714', '100BRA10715', '100BRA10716', '100BRA10717', '100BRA10718', '100BRA10719', '100BRA10720', '100BRA10721', '100BRA10722', '100BRA10723', '100BRA10724', '100BRA10725', '100BRA10728', '100BRA10729', '100BRA10730', '100BRA10731', '100BRA10732', '100BRA10733', '100BRA10734', '100BRA10735', '100BRA10736', '100BRA10737', '100BRA10738', '100BRA10739', '100BRA10740', '100BRA10741', '100BRA10743', '100BRA10744', '100BRA10745', '100BRA10746', '100BRA10747', '100BRA10748', '100BRA10749', '100BRA10751', '100BRA10752', '100BRA10753', '100BRA10754', '100BRA10755', '100BRA10756', '100BRA10757', '100BRA10758', '100BRA10759', '100BRA10760', '100BRA10761', '100BRA10762', '100BRA10763', '100BRA10764', '100BRA10765', '100BRA10766', '100BRA10767', '100BRA10768', '100BRA10769', '100BRA10771', '100BRA10772', '100BRA10773', '100BRA10774', '100BRA10775', '100BRA10776', '100BRA10777', '100BRA10780', '100BRA10781', '100BRA10782', '100BRA10783', '100BRA10784', '100BRA10785', '100BRA10786', '100BRA10787', '100BRA10788', '100BRA10789', '100BRA10790', '100BRA10791', '100BRA10792', '100BRA10793', '100BRA10794', '100BRA10795', '100BRA10796', '100BRA10797', '100BRA10798', '100BRA10799', '100BRA10800', '100BRA10801', '100BRA10802', '100BRA10807', '100BRA10808', '100BRA10809', '100BRA10810', '100BRA10811', '100BRA10812', '100BRA10813', '100BRA10814', '100BRA10815', '100BRA10816', '100BRA10817', '100BRA10818', '100BRA10819', '100BRA10820', '100BRA10821', '100BRA10822', '100BRA10823', '100BRA10831', '100BRA10832', '100BRA10833', '100BRA10834', '100BRA10835', '100BRA10836', '100BRA10837', '100BRA10838', '100BRA10839', '100BRA10840', '100BRA10841', '100BRA10842', '100BRA10843', '100BRA10844', '100BRA10845', '100BRA10846', '100BRA10847', '100BRA10848', '100BRA10849', '100BRA10850', '100BRA10851', '100BRA10852', '100BRA10853', '100BRA10854', '100BRA10855', '100BRA10856', '100BRA10857', '100BRA10858', '100BRA10859', '100BRA10860', '100BRA10861', '100BRA10862', '100BRA10863', '100BRA10864', '100BRA10865', '100BRA10866', '100BRA10867', '100BRA10868', '100BRA10869', '100BRA10870', '100BRA10871', '100BRA10872', '100BRA10873', '100BRA10874', '100BRA10878', '100BRA10879', '100BRA10880', '100BRA10881', '100BRA10882', '100BRA10883', '100BRA10884', '100BRA10885', '100BRA10888', '100BRA10889', '100BRA10890', '100BRA10891', '100BRA10892', '100BRA10893', '100BRA10894', '100BRA10895', '100BRA10896', '100BRA10897', '100BRA10898', '100BRA10903', '100BRA10904', '100BRA10905', '100BRA10906', '100BRA10907', '100BRA10908', '100BRA10909', '100BRA10910', '100BRA10911', '100BRA10915', '100BRA10916', '100BRA10917', '100BRA10918', '100BRA10919', '100BRA10922', '100BRA10923', '100BRA10924', '100BRA10925', '100BRA10926', '100BRA10927', '100BRA10928', '100BRA10929', '100BRA10930', '100BRA10931', '100BRA10932', '100BRA10933', '100BRA10934', '100BRA10935', '100BRA10937', '100BRA10941', '100BRA10942', '100BRA10943', '100BRA10945', '100BRA10946', '100BRA16901', '100BRA16902', '100BRA16903', '100BRA16904', '100BRA16905', '100BRA16906', '100BRA16907', '100BRA16908', '100BRA16910', '100BRA16911', '100BRA16924', '100BRA16925', '100BRA16928', '100BRA16931', '100BRA16933', '100BRA16934', '100BRA16936', '100BRA16938', '100BRA16939', '100BRA16940', '100BRA16942', '100BRA16943', '100BRA16944', '100BRA16946', '100BRA16947', '100BRA46637', '100BRA46638', '100BRA46639', '100BRA46640', '100BRA46641', '100BRA46642', '100BRA46643', '100BRA46644', '100BRA46645', '100BRA46646', '100BRA46647', '100BRA46648', '100BRA46649', '100BRA46650', '100BRA46651', '100BRA46653', '100BRA46654', '100BRA46655', '100BRA46656', '100BRA46657', '100BRA46658', '100BRA56546', '100BRA56547', '100BRA56548', '100BRA56549', '100BRA56550', '100BRA56551', '100BRA56552', '100BRA56553', '100BRA56554', '100BRA56555', '100BRA56556', '100BRA56557', '100BRA56560', '100BRA56561', '100BRA56563', '100BRA56564', '100BRA56565', '100BRA56566', '100BRA56567', '100BRA56568', '100BRA56569', '100BRA56570', '100BRA56572', '100BRA56573', '100BRA56574', '100BRA56575', '100BRA56576', '100BRA56577', '100BRA56578', '100BRA56579', '100BRA56580', '100BRA56581', '100BRC53349', '100BRC53350', '100BRC53351', '100BRC53355', '100BRC53356', '100BRC53357', '100BRC53358', '100BRC53359', '100BRC53363', '100BRC53364', '100BRC53365', '100BRC53367', '100BRC53368', '100BRC53372', '100BRC53374', '100BRC53375', '100BRC53378', '100BRC53380', '100BRC53381', '100BRC53382', '100BRC53383', '100BRC53384', '100BRC53385', '100BRC53386', '100BRC53387', '100BRC53388', '100BRC53390', '100BRC53391', '100BRC53393', '100BRC53394', '100BRC53395', '100BRC53396', '100BRC53397', '100BRC53398', '100BRC53399', '100BRC53400', '100BRC53403', '100BRC53404', '100BRC53405', '100BRC53406', '100BRC53407', '100BRC53408', '100BRP90003', '100BRP90004', '100BRP90008', '100BRP90009', '100BRP90010', '100BRP90011', '100BRP90012', '100BRP90013', '100BRP90015', '100BRP90017', '100BRP90018', '100BRP90019', '100BRP90021', '100BRP90023', '100BRP90025', '100BRP90026', '100BRP90027', '100BRP90028', '100BRP90029', '100BRP90030', '100BRP90031', '100BRP90032', '100BRP90033', '100BRP90034', '100BRP90035', '100BRP90036', '100BRP90037', '100BRP90038', '100BRP90039', '100BRP90040', '100BRP90056', '100BRP90057', '100BRP90058', '100BRP90059', '100BRP90060', '100BRP90061', '100BRP90063', '100BRP90064', '100BRP90065', '100BRP90066', '100BRP90067', '100BRP90068', '100BRP90069', '100BRP90070', '100BRP90071', '100BRP90074', '100BRP90075', '100BRP90076', '100BRP90077', '100BRP90078', '100BRP90079', '100BRP90080', '100BRP90081', '100BRP90082', '100BRP90083', '100BRP90084', '100BRP90085', '100BRP90086', '100BRP90087', '100BRP90088', '100BRP90089', '100BRP90090', '100BRP90091', '100BRP90092', '100BRP90093', '100BRP90094', '100BRP90095', '100BRP90096', '100BRP90097', '100BRP90098', '100BRP90100', '100BRP90101', '100BRP90102', '100BRP90103', '100BRP90104', '100BRP90105', '100BRP90106', '100BRP90107', '100BRP90108', '100BRP90109', '100BRP90110', '100BRP90111', '100BRP90112', '100BRP90114', '100BRP90116', '100BRP90117', '100BRP90118', '100BRP90119', '100BRP90120', '100BRP90121', '100BRP90122', '100BRP90123', '100BRP90124', '100BRP90125', '100BRP90127', '100BRP90128', '100BRP90129', '100BRP90130', '100BRP90131', '100BRP90132', '100BRP90133', '100BRP90134', '100BRP90135', '100BRP90136', '100BRP90137', '100BRP90138', '100BRP90140', '100BRP90141', '100BRP90142', '100BRP90143', '100BRP90145', '100BRP90146', '100BRP90149', '100BRP90150', '100BRP90151', '100BRP90153', '100BRP90154', '100BRP90155', '100BRP90156', '100BRP90157', '100BRP90158', '100BRP90163', '100BRP90165', '100BRP90166', '100BRP90167', '100BRP90168', '100BRP90169', '100BRP90170', '100BRP90171', '100BRP90173', '100BRP90174', '100BRP90175', '100BRP90176', '100BRP90177', '100BRP90178', '100BRP90179', '100BRP90180', '100BRP90181', '100BRP90183', '100BRP90184', '100BRP90185', '100BRP90186', '100BRP90187', '100BRP90188', '100BRP90189', '100BRP90190', '100BRP90191', '100BRP90192', '100BRP90195', '100BRP90196', '100BRP90197', '100BRP90199', '100BRP90200', '100BRP90201', '100BRP90202', '100BRP90203', '100BRP90204', '100BRP90205', '100BRP90206', '100BRP90207', '100BRP90208', '100BRP90210', '100BRP90211', '100BRP90212', '100BRP90213', '100BRP90214', '100BRP90215', '100BRP90216', '100BRP90217', '100BRP90218', '100BRP90219', '100BRP90221', '100BRP90224', '100BRP90225', '100BRP90226', '100BRP90227', '100BRP90228', '100BRP90231', '100BRP90232', '100BRP90233', '100BRP90234', '100BRP90235', '100BRP90236', '100BRP90237', '100BRP90268', '100BRP90269', '100BRP90270', '100BRP90271', '100BRP90272', '100BRP90273', '100BRP90307', '100BRP90308', '100BRP90309', '100BRP90310', '100BRP90311', '100BRP90312', '100BRP90313', '100BRP90317', '100BRP90318', '100BRP90319', '100BRP90320', '100BRP90324', '100BRP90325', '100BRP90326', '100BRP90327', '100BRP90328', '100BRP90329', '100BRP90330', '100BRP90332', '100BRP90333', '100BRP90335', '100BRP90336', '100BRP90337', '100BRP90338', '100BRP90339', '100BRP90340', '100BRP90341', '100BRP90342', '100BRP90343', '100BRP90344', '100BRP90345', '100BRP90346', '100BRP90347', '100BRP90348', '100BRP90349', '100BRP90350', '100BRP90354', '100BRP90355', '100BRP90356', '100BRP90357', '100BRP90363', '100BRP90364', '100BRP90365', '100BRP90366', '100BRP90368', '100BRP90369', '100BRP90371', '100BRP90372', '100BRP90373', '100BRP90377', '100BRP90378', '100BRP90379', '100BRP90380', '100BRP90381', '100BRP90382', '100BRP90383', '100BRP90384', '100BRP90385', '100BRP90386', '100BRP90387', '100BRP90388', '100BRP90396', '100BRP90399', '100BRP90402', '100BRP90404', '100BRP90405', '100BRP90408', '100BRP90409', '100BRP90671', '100BRP90673', '100BRP90674', '100BRP90675', '100BRP90676', '100BRP90677', '100BRP90678', '100BRP90979', '100BRP90981', '100BRP90982', '100BRP90983', '100BRP90984', '100BRP90986', '100BRP90987', '100BRP90988', '100BRP90989', '100BRP90990', '100BRP90991', '100BRP90996', '100BRP90997', '100BRP90998', '100BRP90999', '100BRP91001', '100BRP91002', '100BRP91003', '100BRP91004', '100BRP91005', '100BRP91006', '100BRP91008', '100BRP91011', '100BRP91012', '100BRP91013', '100BRP91014', '100BRP91015', '100BRP91016', '100BRP91017', '100BRP91018', '100BRP91019', '100BRP91020', '100BRP91021', '100BRP91022', '100BRP91023', '100BRP91024', '100BRP91027', '100BRP91028', '100BRP91029', '100BRP91030', '100BRP91031', '100BRP91032', '100BRP91033', '100BRP91034', '100BRP91035', '100BRP91036', '100BRP91037', '100BRP91038', '100BRP91039', '100BRP91040', '100BRP91041', '100BRP91042', '100BRP91043', '100BRP91044', '100BRP91045', '100BRP91046', '100BRP91047', '100BRP91048', '100BRP91049', '100BRP91050', '100BRP91051', '100BRP91052', '100BRP91053', '100BRP91054', '100BRP91055', '100BRP91057', '100BRP91058', '100BRP91059', '100BRP91060', '100BRP91061', '100BRP91062', '100BRP91063', '100BRP91064', '100BRP91065', '100BRP91066', '100BRP91067', '100BRP91068', '100BRP91071', '100BRP91072', '100BRP91073', '100BRP91074', '100BRP91075', '100BRP91076', '100BRP91077', '100BRP91078', '100BRP91080', '100BRP91081', '100BRP91082', '100BRP91083', '100BRP91084', '100BRP91085', '100BRP91086', '100BRP91087', '100BRP91088', '100BRP91089', '100BRP91090', '100BRP91091', '100BRP91092', '100BRP91093', '100BRP91094', '100BRP91095', '100BRP91096', '100BRP91097', '100BRP91098', '100BRP91099', '100BRP91100', '100BRP91102', '100BRP91103', '100BRP91104', '100BRP91105', '100BRP91106', '100BRP91107', '100BRP91108', '100BRP91109', '100BRP91112', '100BRP91113', '100BRP91114', '100BRP91115', '100BRP92000', '100BRP92001', '100BRP92002', '100BRP92003', '100BRP92004', '100BRP92005', '100BRP92006', '100BRP92007', '100BRP92008', '100BRP92009', '100BRP92010', '100BRP92011', '100BRP92012', '100BRP92013', '100BRP92014', '100BRP92015', '100BRP92016', '100BRP92017', '100BRP92018', '100BRP92019', '100BRP92020', '100BRP92021', '100BRP92022', '100BRP92023', '100BRP92024', '100BRP92025', '100BRP92026', '100BRP92027', '100BRP92028', '100BRP92029', '100BRP92030', '100BRP92031', '100BRP92032', '100BRP92033', '100BRP92034', '100BRP92035', '100BRP92036', '100BRP92037', '100BRP92038', '100BRP92039', '100BRP92040', '100BRP92041', '100BRP92042', '100BRP92043', '100BRP92044', '100BRP92045', '100BRP92046', '100BRP92047', '100BRP92048', '100BRP92049', '100BRP92050', '100BRP92051', '100BRP92052', '100BRP92053', '100BRP92054', '100BRP92055', '100BRP92056', '100BRP92057', '100BRP92058', '100BRP92059', '100BRP92060', '100BRP92061', '100BRP92062', '100BRP92063', '100BRP92064', '100BRP92065', '100BRP92066', '100BRP92067', '100BRP92068', '100BRP92069', '100BRP92071', '100BRP92072', '100BRP92073', '100BRP92074', '100BRP92075', '100BRP92076', '100BRP92077', '100BRP92078', '100BRP92079', '100BRP92080', '100BRP92081', '100BRP92082', '100BRX32920', '100BRX32921', '100BRX32922', '100BRX43052', '100BRX43055', '100BRZ00678', '100BRZ00681', '100BRZ00686', '100BRZ00687', '100BRZ00692', '100BRZ00694', '100BRZ00695', '100BRZ00696', '100BRZ00698', '100BRZ00699', '100BRZ00702', '100BRZ00703', '100BRZ00704', '100BRZ00705', '100BRZ01655', '100BRZ01656', '100BRZ01657', '100BRZ01658', '100BRZ01659', '100BRZ01660', '100BRZ01661', '100BRZ01662', '100BRZ01663', '100BRZ01664', '100BRZ01665', '100BRZ01666', '100BRZ01667', '100BRZ01668', '100BRZ01669', '100BRZ01670', '100BRZ01671', '100BRZ01672', '100BRZ01673', '100BRZ01674', '100BRZ01675', '100BRZ01676', '100BRZ01677', '100BRZ01678', '100BRZ01679', '100BRZ01680', '100BRZ01682', '100BRZ01683', '100BRZ01684', '100BRZ01685', '100BRZ01686', '100BRZ01687', '100BRZ01688', '100BRZ01689', '100BRZ01690', '100BRZ01691', '100BRZ01692', '100BRZ01693', '100BRZ01694', '100BRZ01695', '100BRZ01696', '100BRZ01697', '100BRZ01699', '100BRZ01700', '100BRZ01701', '100BRZ01707', '100BRZ01708', '100BRZ01709', '100BRZ01710', '100BRZ01713', '100FBX18331', '100FBX18336', '100FBX18337', '100FBX18339', '100FBX18342', '100SGB20368', '100SGP90563', '100SGY38500', '100SGZ01485', '170BRP91110', '170BRP91111', '190SBX18338']</t>
+          <t>['0100BAC30684', '0100BAC30685', '0100BAC30742', '0100BAC30743', '0100BAC30946', '0100BAZ02458', '0100BAZ02459', '0100BRA01797', '0100BRA01798', '0100BRA01799', '0100BRA01800', '0100BRA10006', '0100BRA10007', '0100BRA10008', '0100BRA10009', '0100BRA10010', '0100BRA10011', '0100BRA10012', '0100BRA10013', '0100BRA10014', '0100BRA10015', '0100BRA10016', '0100BRA10021', '0100BRA10022', '0100BRA10023', '0100BRA10024', '0100BRA10025', '0100BRA10026', '0100BRA10027', '0100BRA10029', '0100BRA10030', '0100BRA10031', '0100BRA10032', '0100BRA10033', '0100BRA10034', '0100BRA10035', '0100BRA10036', '0100BRA10037', '0100BRA10038', '0100BRA10039', '0100BRA10040', '0100BRA10041', '0100BRA10042', '0100BRA10047', '0100BRA10048', '0100BRA10049', '0100BRA10050', '0100BRA10051', '0100BRA10052', '0100BRA10053', '0100BRA10054', '0100BRA10055', '0100BRA10056', '0100BRA10057', '0100BRA10059', '0100BRA10062', '0100BRA10064', '0100BRA10065', '0100BRA10066', '0100BRA10067', '0100BRA10068', '0100BRA10069', '0100BRA10070', '0100BRA10071', '0100BRA10072', '0100BRA10073', '0100BRA10074', '0100BRA10075', '0100BRA10076', '0100BRA10077', '0100BRA10078', '0100BRA10079', '0100BRA10080', '0100BRA10081', '0100BRA10082', '0100BRA10083', '0100BRA10084', '0100BRA10086', '0100BRA10087', '0100BRA10088', '0100BRA10089', '0100BRA10090', '0100BRA10091', '0100BRA10092', '0100BRA10093', '0100BRA10094', '0100BRA10095', '0100BRA10096', '0100BRA10097', '0100BRA10098', '0100BRA10099', '0100BRA10100', '0100BRA10101', '0100BRA10102', '0100BRA10103', '0100BRA10104', '0100BRA10105', '0100BRA10106', '0100BRA10107', '0100BRA10108', '0100BRA10109', '0100BRA10110', '0100BRA10111', '0100BRA10112', '0100BRA10113', '0100BRA10114', '0100BRA10115', '0100BRA10116', '0100BRA10117', '0100BRA10119', '0100BRA10120', '0100BRA10121', '0100BRA10122', '0100BRA10123', '0100BRA10124', '0100BRA10125', '0100BRA10126', '0100BRA10127', '0100BRA10128', '0100BRA10129', '0100BRA10130', '0100BRA10131', '0100BRA10132', '0100BRA10133', '0100BRA10134', '0100BRA10135', '0100BRA10136', '0100BRA10137', '0100BRA10138', '0100BRA10139', '0100BRA10140', '0100BRA10143', '0100BRA10144', '0100BRA10145', '0100BRA10146', '0100BRA10147', '0100BRA10148', '0100BRA10149', '0100BRA10150', '0100BRA10151', '0100BRA10152', '0100BRA10153', '0100BRA10154', '0100BRA10155', '0100BRA10156', '0100BRA10157', '0100BRA10158', '0100BRA10159', '0100BRA10160', '0100BRA10161', '0100BRA10162', '0100BRA10163', '0100BRA10164', '0100BRA10165', '0100BRA10166', '0100BRA10167', '0100BRA10168', '0100BRA10169', '0100BRA10170', '0100BRA10171', '0100BRA10172', '0100BRA10173', '0100BRA10174', '0100BRA10175', '0100BRA10176', '0100BRA10177', '0100BRA10178', '0100BRA10179', '0100BRA10180', '0100BRA10181', '0100BRA10182', '0100BRA10183', '0100BRA10184', '0100BRA10187', '0100BRA10188', '0100BRA10189', '0100BRA10190', '0100BRA10191', '0100BRA10192', '0100BRA10193', '0100BRA10195', '0100BRA10196', '0100BRA10197', '0100BRA10198', '0100BRA10199', '0100BRA10200', '0100BRA10201', '0100BRA10202', '0100BRA10203', '0100BRA10204', '0100BRA10205', '0100BRA10206', '0100BRA10207', '0100BRA10208', '0100BRA10209', '0100BRA10210', '0100BRA10211', '0100BRA10212', '0100BRA10213', '0100BRA10214', '0100BRA10215', '0100BRA10216', '0100BRA10217', '0100BRA10218', '0100BRA10219', '0100BRA10220', '0100BRA10221', '0100BRA10225', '0100BRA10229', '0100BRA10230', '0100BRA10231', '0100BRA10233', '0100BRA10235', '0100BRA10236', '0100BRA10237', '0100BRA10238', '0100BRA10239', '0100BRA10240', '0100BRA10241', '0100BRA10242', '0100BRA10243', '0100BRA10244', '0100BRA10245', '0100BRA10246', '0100BRA10247', '0100BRA10248', '0100BRA10249', '0100BRA10250', '0100BRA10251', '0100BRA10252', '0100BRA10253', '0100BRA10254', '0100BRA10255', '0100BRA10256', '0100BRA10257', '0100BRA10258', '0100BRA10259', '0100BRA10260', '0100BRA10261', '0100BRA10262', '0100BRA10263', '0100BRA10264', '0100BRA10265', '0100BRA10266', '0100BRA10267', '0100BRA10269', '0100BRA10270', '0100BRA10272', '0100BRA10273', '0100BRA10274', '0100BRA10275', '0100BRA10276', '0100BRA10277', '0100BRA10278', '0100BRA10279', '0100BRA10280', '0100BRA10281', '0100BRA10282', '0100BRA10283', '0100BRA10284', '0100BRA10285', '0100BRA10286', '0100BRA10287', '0100BRA10288', '0100BRA10289', '0100BRA10290', '0100BRA10291', '0100BRA10292', '0100BRA10293', '0100BRA10294', '0100BRA10295', '0100BRA10296', '0100BRA10297', '0100BRA10298', '0100BRA10299', '0100BRA10300', '0100BRA10301', '0100BRA10302', '0100BRA10303', '0100BRA10304', '0100BRA10305', '0100BRA10306', '0100BRA10308', '0100BRA10309', '0100BRA10311', '0100BRA10312', '0100BRA10313', '0100BRA10315', '0100BRA10316', '0100BRA10317', '0100BRA10318', '0100BRA10319', '0100BRA10320', '0100BRA10321', '0100BRA10323', '0100BRA10324', '0100BRA10325', '0100BRA10326', '0100BRA10327', '0100BRA10328', '0100BRA10329', '0100BRA10330', '0100BRA10331', '0100BRA10332', '0100BRA10333', '0100BRA10334', '0100BRA10335', '0100BRA10336', '0100BRA10337', '0100BRA10339', '0100BRA10340', '0100BRA10342', '0100BRA10343', '0100BRA10344', '0100BRA10352', '0100BRA10353', '0100BRA10354', '0100BRA10355', '0100BRA10356', '0100BRA10357', '0100BRA10358', '0100BRA10359', '0100BRA10360', '0100BRA10361', '0100BRA10362', '0100BRA10363', '0100BRA10364', '0100BRA10365', '0100BRA10366', '0100BRA10367', '0100BRA10368', '0100BRA10369', '0100BRA10370', '0100BRA10371', '0100BRA10372', '0100BRA10373', '0100BRA10374', '0100BRA10375', '0100BRA10376', '0100BRA10377', '0100BRA10378', '0100BRA10381', '0100BRA10382', '0100BRA10383', '0100BRA10384', '0100BRA10385', '0100BRA10386', '0100BRA10392', '0100BRA10393', '0100BRA10394', '0100BRA10395', '0100BRA10396', '0100BRA10397', '0100BRA10398', '0100BRA10399', '0100BRA10400', '0100BRA10401', '0100BRA10403', '0100BRA10404', '0100BRA10405', '0100BRA10406', '0100BRA10407', '0100BRA10408', '0100BRA10409', '0100BRA10410', '0100BRA10411', '0100BRA10412', '0100BRA10413', '0100BRA10414', '0100BRA10415', '0100BRA10417', '0100BRA10418', '0100BRA10419', '0100BRA10421', '0100BRA10423', '0100BRA10425', '0100BRA10426', '0100BRA10427', '0100BRA10428', '0100BRA10429', '0100BRA10430', '0100BRA10431', '0100BRA10432', '0100BRA10433', '0100BRA10434', '0100BRA10435', '0100BRA10436', '0100BRA10437', '0100BRA10438', '0100BRA10439', '0100BRA10440', '0100BRA10441', '0100BRA10442', '0100BRA10443', '0100BRA10444', '0100BRA10445', '0100BRA10446', '0100BRA10447', '0100BRA10448', '0100BRA10449', '0100BRA10450', '0100BRA10451', '0100BRA10452', '0100BRA10453', '0100BRA10454', '0100BRA10455', '0100BRA10456', '0100BRA10457', '0100BRA10458', '0100BRA10459', '0100BRA10460', '0100BRA10461', '0100BRA10464', '0100BRA10465', '0100BRA10466', '0100BRA10467', '0100BRA10468', '0100BRA10469', '0100BRA10470', '0100BRA10471', '0100BRA10472', '0100BRA10473', '0100BRA10474', '0100BRA10475', '0100BRA10476', '0100BRA10477', '0100BRA10478', '0100BRA10479', '0100BRA10480', '0100BRA10481', '0100BRA10482', '0100BRA10483', '0100BRA10484', '0100BRA10485', '0100BRA10486', '0100BRA10487', '0100BRA10488', '0100BRA10489', '0100BRA10490', '0100BRA10491', '0100BRA10492', '0100BRA10493', '0100BRA10494', '0100BRA10495', '0100BRA10496', '0100BRA10497', '0100BRA10498', '0100BRA10499', '0100BRA10500', '0100BRA10501', '0100BRA10502', '0100BRA10503', '0100BRA10504', '0100BRA10505', '0100BRA10506', '0100BRA10507', '0100BRA10508', '0100BRA10509', '0100BRA10510', '0100BRA10511', '0100BRA10512', '0100BRA10513', '0100BRA10514', '0100BRA10515', '0100BRA10516', '0100BRA10521', '0100BRA10522', '0100BRA10523', '0100BRA10524', '0100BRA10525', '0100BRA10527', '0100BRA10528', '0100BRA10529', '0100BRA10530', '0100BRA10531', '0100BRA10532', '0100BRA10533', '0100BRA10534', '0100BRA10535', '0100BRA10536', '0100BRA10537', '0100BRA10538', '0100BRA10539', '0100BRA10540', '0100BRA10543', '0100BRA10544', '0100BRA10545', '0100BRA10546', '0100BRA10547', '0100BRA10548', '0100BRA10549', '0100BRA10550', '0100BRA10551', '0100BRA10553', '0100BRA10554', '0100BRA10555', '0100BRA10556', '0100BRA10557', '0100BRA10558', '0100BRA10559', '0100BRA10560', '0100BRA10561', '0100BRA10562', '0100BRA10563', '0100BRA10564', '0100BRA10565', '0100BRA10566', '0100BRA10567', '0100BRA10570', '0100BRA10571', '0100BRA10572', '0100BRA10574', '0100BRA10575', '0100BRA10576', '0100BRA10577', '0100BRA10578', '0100BRA10579', '0100BRA10580', '0100BRA10583', '0100BRA10584', '0100BRA10585', '0100BRA10586', '0100BRA10587', '0100BRA10588', '0100BRA10589', '0100BRA10590', '0100BRA10591', '0100BRA10592', '0100BRA10593', '0100BRA10594', '0100BRA10595', '0100BRA10596', '0100BRA10598', '0100BRA10599', '0100BRA10600', '0100BRA10601', '0100BRA10602', '0100BRA10603', '0100BRA10604', '0100BRA10605', '0100BRA10606', '0100BRA10607', '0100BRA10608', '0100BRA10609', '0100BRA10614', '0100BRA10616', '0100BRA10617', '0100BRA10618', '0100BRA10619', '0100BRA10620', '0100BRA10621', '0100BRA10622', '0100BRA10623', '0100BRA10624', '0100BRA10625', '0100BRA10626', '0100BRA10627', '0100BRA10628', '0100BRA10629', '0100BRA10630', '0100BRA10631', '0100BRA10632', '0100BRA10633', '0100BRA10634', '0100BRA10635', '0100BRA10636', '0100BRA10637', '0100BRA10638', '0100BRA10639', '0100BRA10640', '0100BRA10641', '0100BRA10642', '0100BRA10643', '0100BRA10644', '0100BRA10645', '0100BRA10647', '0100BRA10648', '0100BRA10649', '0100BRA10650', '0100BRA10651', '0100BRA10652', '0100BRA10653', '0100BRA10654', '0100BRA10655', '0100BRA10656', '0100BRA10657', '0100BRA10658', '0100BRA10659', '0100BRA10660', '0100BRA10661', '0100BRA10662', '0100BRA10663', '0100BRA10665', '0100BRA10666', '0100BRA10667', '0100BRA10668', '0100BRA10669', '0100BRA10673', '0100BRA10674', '0100BRA10675', '0100BRA10676', '0100BRA10677', '0100BRA10678', '0100BRA10679', '0100BRA10680', '0100BRA10681', '0100BRA10682', '0100BRA10683', '0100BRA10684', '0100BRA10685', '0100BRA10686', '0100BRA10687', '0100BRA10691', '0100BRA10692', '0100BRA10693', '0100BRA10696', '0100BRA10697', '0100BRA10698', '0100BRA10699', '0100BRA10700', '0100BRA10701', '0100BRA10702', '0100BRA10703', '0100BRA10704', '0100BRA10706', '0100BRA10707', '0100BRA10708', '0100BRA10709', '0100BRA10710', '0100BRA10711', '0100BRA10712', '0100BRA10713', '0100BRA10714', '0100BRA10715', '0100BRA10716', '0100BRA10717', '0100BRA10718', '0100BRA10719', '0100BRA10720', '0100BRA10721', '0100BRA10722', '0100BRA10723', '0100BRA10724', '0100BRA10725', '0100BRA10728', '0100BRA10729', '0100BRA10730', '0100BRA10731', '0100BRA10732', '0100BRA10733', '0100BRA10734', '0100BRA10735', '0100BRA10736', '0100BRA10737', '0100BRA10738', '0100BRA10739', '0100BRA10740', '0100BRA10741', '0100BRA10743', '0100BRA10744', '0100BRA10745', '0100BRA10746', '0100BRA10747', '0100BRA10748', '0100BRA10749', '0100BRA10751', '0100BRA10752', '0100BRA10753', '0100BRA10754', '0100BRA10755', '0100BRA10756', '0100BRA10757', '0100BRA10758', '0100BRA10759', '0100BRA10760', '0100BRA10761', '0100BRA10762', '0100BRA10763', '0100BRA10764', '0100BRA10765', '0100BRA10766', '0100BRA10767', '0100BRA10768', '0100BRA10769', '0100BRA10771', '0100BRA10772', '0100BRA10773', '0100BRA10774', '0100BRA10775', '0100BRA10776', '0100BRA10777', '0100BRA10780', '0100BRA10781', '0100BRA10782', '0100BRA10783', '0100BRA10784', '0100BRA10785', '0100BRA10786', '0100BRA10787', '0100BRA10788', '0100BRA10789', '0100BRA10790', '0100BRA10791', '0100BRA10792', '0100BRA10793', '0100BRA10794', '0100BRA10795', '0100BRA10796', '0100BRA10797', '0100BRA10798', '0100BRA10799', '0100BRA10800', '0100BRA10801', '0100BRA10802', '0100BRA10807', '0100BRA10808', '0100BRA10809', '0100BRA10810', '0100BRA10811', '0100BRA10812', '0100BRA10813', '0100BRA10814', '0100BRA10815', '0100BRA10816', '0100BRA10817', '0100BRA10818', '0100BRA10819', '0100BRA10820', '0100BRA10821', '0100BRA10822', '0100BRA10823', '0100BRA10831', '0100BRA10832', '0100BRA10833', '0100BRA10834', '0100BRA10835', '0100BRA10836', '0100BRA10837', '0100BRA10838', '0100BRA10839', '0100BRA10840', '0100BRA10841', '0100BRA10842', '0100BRA10843', '0100BRA10844', '0100BRA10845', '0100BRA10846', '0100BRA10847', '0100BRA10848', '0100BRA10849', '0100BRA10850', '0100BRA10851', '0100BRA10852', '0100BRA10853', '0100BRA10854', '0100BRA10855', '0100BRA10856', '0100BRA10857', '0100BRA10858', '0100BRA10859', '0100BRA10860', '0100BRA10861', '0100BRA10862', '0100BRA10863', '0100BRA10864', '0100BRA10865', '0100BRA10866', '0100BRA10867', '0100BRA10868', '0100BRA10869', '0100BRA10870', '0100BRA10871', '0100BRA10872', '0100BRA10873', '0100BRA10874', '0100BRA10878', '0100BRA10879', '0100BRA10880', '0100BRA10881', '0100BRA10882', '0100BRA10883', '0100BRA10884', '0100BRA10885', '0100BRA10888', '0100BRA10889', '0100BRA10890', '0100BRA10891', '0100BRA10892', '0100BRA10893', '0100BRA10894', '0100BRA10895', '0100BRA10896', '0100BRA10897', '0100BRA10898', '0100BRA10903', '0100BRA10904', '0100BRA10905', '0100BRA10906', '0100BRA10907', '0100BRA10908', '0100BRA10909', '0100BRA10910', '0100BRA10911', '0100BRA10915', '0100BRA10916', '0100BRA10917', '0100BRA10918', '0100BRA10919', '0100BRA10922', '0100BRA10923', '0100BRA10924', '0100BRA10925', '0100BRA10926', '0100BRA10927', '0100BRA10928', '0100BRA10929', '0100BRA10930', '0100BRA10931', '0100BRA10932', '0100BRA10933', '0100BRA10934', '0100BRA10935', '0100BRA10937', '0100BRA10941', '0100BRA10942', '0100BRA10943', '0100BRA10945', '0100BRA10946', '0100BRA16901', '0100BRA16902', '0100BRA16903', '0100BRA16904', '0100BRA16905', '0100BRA16906', '0100BRA16907', '0100BRA16908', '0100BRA16910', '0100BRA16911', '0100BRA16924', '0100BRA16925', '0100BRA16928', '0100BRA16931', '0100BRA16933', '0100BRA16934', '0100BRA16936', '0100BRA16938', '0100BRA16939', '0100BRA16940', '0100BRA16942', '0100BRA16943', '0100BRA16944', '0100BRA16946', '0100BRA16947', '0100BRA46637', '0100BRA46638', '0100BRA46639', '0100BRA46640', '0100BRA46641', '0100BRA46642', '0100BRA46643', '0100BRA46644', '0100BRA46645', '0100BRA46646', '0100BRA46647', '0100BRA46648', '0100BRA46649', '0100BRA46650', '0100BRA46651', '0100BRA46653', '0100BRA46654', '0100BRA46655', '0100BRA46656', '0100BRA46657', '0100BRA46658', '0100BRA56546', '0100BRA56547', '0100BRA56548', '0100BRA56549', '0100BRA56550', '0100BRA56551', '0100BRA56552', '0100BRA56553', '0100BRA56554', '0100BRA56555', '0100BRA56556', '0100BRA56557', '0100BRA56560', '0100BRA56561', '0100BRA56563', '0100BRA56564', '0100BRA56565', '0100BRA56566', '0100BRA56567', '0100BRA56568', '0100BRA56569', '0100BRA56570', '0100BRA56572', '0100BRA56573', '0100BRA56574', '0100BRA56575', '0100BRA56576', '0100BRA56577', '0100BRA56578', '0100BRA56579', '0100BRA56580', '0100BRA56581', '0100BRC53349', '0100BRC53350', '0100BRC53351', '0100BRC53355', '0100BRC53356', '0100BRC53357', '0100BRC53358', '0100BRC53359', '0100BRC53363', '0100BRC53364', '0100BRC53365', '0100BRC53367', '0100BRC53368', '0100BRC53372', '0100BRC53374', '0100BRC53375', '0100BRC53378', '0100BRC53380', '0100BRC53381', '0100BRC53382', '0100BRC53383', '0100BRC53384', '0100BRC53385', '0100BRC53386', '0100BRC53387', '0100BRC53388', '0100BRC53390', '0100BRC53391', '0100BRC53393', '0100BRC53394', '0100BRC53395', '0100BRC53396', '0100BRC53397', '0100BRC53398', '0100BRC53399', '0100BRC53400', '0100BRC53403', '0100BRC53404', '0100BRC53405', '0100BRC53406', '0100BRC53407', '0100BRC53408', '0100BRP90003', '0100BRP90004', '0100BRP90008', '0100BRP90009', '0100BRP90010', '0100BRP90011', '0100BRP90012', '0100BRP90013', '0100BRP90015', '0100BRP90017', '0100BRP90018', '0100BRP90019', '0100BRP90021', '0100BRP90023', '0100BRP90025', '0100BRP90026', '0100BRP90027', '0100BRP90028', '0100BRP90029', '0100BRP90030', '0100BRP90031', '0100BRP90032', '0100BRP90033', '0100BRP90034', '0100BRP90035', '0100BRP90036', '0100BRP90037', '0100BRP90038', '0100BRP90039', '0100BRP90040', '0100BRP90056', '0100BRP90057', '0100BRP90058', '0100BRP90059', '0100BRP90060', '0100BRP90061', '0100BRP90063', '0100BRP90064', '0100BRP90065', '0100BRP90066', '0100BRP90067', '0100BRP90068', '0100BRP90069', '0100BRP90070', '0100BRP90071', '0100BRP90074', '0100BRP90075', '0100BRP90076', '0100BRP90077', '0100BRP90078', '0100BRP90079', '0100BRP90080', '0100BRP90081', '0100BRP90082', '0100BRP90083', '0100BRP90084', '0100BRP90085', '0100BRP90086', '0100BRP90087', '0100BRP90088', '0100BRP90089', '0100BRP90090', '0100BRP90091', '0100BRP90092', '0100BRP90093', '0100BRP90094', '0100BRP90095', '0100BRP90096', '0100BRP90097', '0100BRP90098', '0100BRP90100', '0100BRP90101', '0100BRP90102', '0100BRP90103', '0100BRP90104', '0100BRP90105', '0100BRP90106', '0100BRP90107', '0100BRP90108', '0100BRP90109', '0100BRP90110', '0100BRP90111', '0100BRP90112', '0100BRP90114', '0100BRP90116', '0100BRP90117', '0100BRP90118', '0100BRP90119', '0100BRP90120', '0100BRP90121', '0100BRP90122', '0100BRP90123', '0100BRP90124', '0100BRP90125', '0100BRP90127', '0100BRP90128', '0100BRP90129', '0100BRP90130', '0100BRP90131', '0100BRP90132', '0100BRP90133', '0100BRP90134', '0100BRP90135', '0100BRP90136', '0100BRP90137', '0100BRP90138', '0100BRP90140', '0100BRP90141', '0100BRP90142', '0100BRP90143', '0100BRP90145', '0100BRP90146', '0100BRP90149', '0100BRP90150', '0100BRP90151', '0100BRP90153', '0100BRP90154', '0100BRP90155', '0100BRP90156', '0100BRP90157', '0100BRP90158', '0100BRP90163', '0100BRP90165', '0100BRP90166', '0100BRP90167', '0100BRP90168', '0100BRP90169', '0100BRP90170', '0100BRP90171', '0100BRP90173', '0100BRP90174', '0100BRP90175', '0100BRP90176', '0100BRP90177', '0100BRP90178', '0100BRP90179', '0100BRP90180', '0100BRP90181', '0100BRP90183', '0100BRP90184', '0100BRP90185', '0100BRP90186', '0100BRP90187', '0100BRP90188', '0100BRP90189', '0100BRP90190', '0100BRP90191', '0100BRP90192', '0100BRP90195', '0100BRP90196', '0100BRP90197', '0100BRP90199', '0100BRP90200', '0100BRP90201', '0100BRP90202', '0100BRP90203', '0100BRP90204', '0100BRP90205', '0100BRP90206', '0100BRP90207', '0100BRP90208', '0100BRP90210', '0100BRP90211', '0100BRP90212', '0100BRP90213', '0100BRP90214', '0100BRP90215', '0100BRP90216', '0100BRP90217', '0100BRP90218', '0100BRP90219', '0100BRP90221', '0100BRP90224', '0100BRP90225', '0100BRP90226', '0100BRP90227', '0100BRP90228', '0100BRP90231', '0100BRP90232', '0100BRP90233', '0100BRP90234', '0100BRP90235', '0100BRP90236', '0100BRP90237', '0100BRP90268', '0100BRP90269', '0100BRP90270', '0100BRP90271', '0100BRP90272', '0100BRP90273', '0100BRP90307', '0100BRP90308', '0100BRP90309', '0100BRP90310', '0100BRP90311', '0100BRP90312', '0100BRP90313', '0100BRP90317', '0100BRP90318', '0100BRP90319', '0100BRP90320', '0100BRP90324', '0100BRP90325', '0100BRP90326', '0100BRP90327', '0100BRP90328', '0100BRP90329', '0100BRP90330', '0100BRP90332', '0100BRP90333', '0100BRP90335', '0100BRP90336', '0100BRP90337', '0100BRP90338', '0100BRP90339', '0100BRP90340', '0100BRP90341', '0100BRP90342', '0100BRP90343', '0100BRP90344', '0100BRP90345', '0100BRP90346', '0100BRP90347', '0100BRP90348', '0100BRP90349', '0100BRP90350', '0100BRP90354', '0100BRP90355', '0100BRP90356', '0100BRP90357', '0100BRP90363', '0100BRP90364', '0100BRP90365', '0100BRP90366', '0100BRP90368', '0100BRP90369', '0100BRP90371', '0100BRP90372', '0100BRP90373', '0100BRP90377', '0100BRP90378', '0100BRP90379', '0100BRP90380', '0100BRP90381', '0100BRP90382', '0100BRP90383', '0100BRP90384', '0100BRP90385', '0100BRP90386', '0100BRP90387', '0100BRP90388', '0100BRP90396', '0100BRP90399', '0100BRP90402', '0100BRP90404', '0100BRP90405', '0100BRP90408', '0100BRP90409', '0100BRP90671', '0100BRP90673', '0100BRP90674', '0100BRP90675', '0100BRP90676', '0100BRP90677', '0100BRP90678', '0100BRP90979', '0100BRP90981', '0100BRP90982', '0100BRP90983', '0100BRP90984', '0100BRP90986', '0100BRP90987', '0100BRP90988', '0100BRP90989', '0100BRP90990', '0100BRP90991', '0100BRP90996', '0100BRP90997', '0100BRP90998', '0100BRP90999', '0100BRP91001', '0100BRP91002', '0100BRP91003', '0100BRP91004', '0100BRP91005', '0100BRP91006', '0100BRP91008', '0100BRP91011', '0100BRP91012', '0100BRP91013', '0100BRP91014', '0100BRP91015', '0100BRP91016', '0100BRP91017', '0100BRP91018', '0100BRP91019', '0100BRP91020', '0100BRP91021', '0100BRP91022', '0100BRP91023', '0100BRP91024', '0100BRP91027', '0100BRP91028', '0100BRP91029', '0100BRP91030', '0100BRP91031', '0100BRP91032', '0100BRP91033', '0100BRP91034', '0100BRP91035', '0100BRP91036', '0100BRP91037', '0100BRP91038', '0100BRP91039', '0100BRP91040', '0100BRP91041', '0100BRP91042', '0100BRP91043', '0100BRP91044', '0100BRP91045', '0100BRP91046', '0100BRP91047', '0100BRP91048', '0100BRP91049', '0100BRP91050', '0100BRP91051', '0100BRP91052', '0100BRP91053', '0100BRP91054', '0100BRP91055', '0100BRP91057', '0100BRP91058', '0100BRP91059', '0100BRP91060', '0100BRP91061', '0100BRP91062', '0100BRP91063', '0100BRP91064', '0100BRP91065', '0100BRP91066', '0100BRP91067', '0100BRP91068', '0100BRP91071', '0100BRP91072', '0100BRP91073', '0100BRP91074', '0100BRP91075', '0100BRP91076', '0100BRP91077', '0100BRP91078', '0100BRP91080', '0100BRP91081', '0100BRP91082', '0100BRP91083', '0100BRP91084', '0100BRP91085', '0100BRP91086', '0100BRP91087', '0100BRP91088', '0100BRP91089', '0100BRP91090', '0100BRP91091', '0100BRP91092', '0100BRP91093', '0100BRP91094', '0100BRP91095', '0100BRP91096', '0100BRP91097', '0100BRP91098', '0100BRP91099', '0100BRP91100', '0100BRP91102', '0100BRP91103', '0100BRP91104', '0100BRP91105', '0100BRP91106', '0100BRP91107', '0100BRP91108', '0100BRP91109', '0100BRP91112', '0100BRP91113', '0100BRP91114', '0100BRP91115', '0100BRP92000', '0100BRP92001', '0100BRP92002', '0100BRP92003', '0100BRP92004', '0100BRP92005', '0100BRP92006', '0100BRP92007', '0100BRP92008', '0100BRP92009', '0100BRP92010', '0100BRP92011', '0100BRP92012', '0100BRP92013', '0100BRP92014', '0100BRP92015', '0100BRP92016', '0100BRP92017', '0100BRP92018', '0100BRP92019', '0100BRP92020', '0100BRP92021', '0100BRP92022', '0100BRP92023', '0100BRP92024', '0100BRP92025', '0100BRP92026', '0100BRP92027', '0100BRP92028', '0100BRP92029', '0100BRP92030', '0100BRP92031', '0100BRP92032', '0100BRP92033', '0100BRP92034', '0100BRP92035', '0100BRP92036', '0100BRP92037', '0100BRP92038', '0100BRP92039', '0100BRP92040', '0100BRP92041', '0100BRP92042', '0100BRP92043', '0100BRP92044', '0100BRP92045', '0100BRP92046', '0100BRP92047', '0100BRP92048', '0100BRP92049', '0100BRP92050', '0100BRP92051', '0100BRP92052', '0100BRP92053', '0100BRP92054', '0100BRP92055', '0100BRP92056', '0100BRP92057', '0100BRP92058', '0100BRP92059', '0100BRP92060', '0100BRP92061', '0100BRP92062', '0100BRP92063', '0100BRP92064', '0100BRP92065', '0100BRP92066', '0100BRP92067', '0100BRP92068', '0100BRP92069', '0100BRP92071', '0100BRP92072', '0100BRP92073', '0100BRP92074', '0100BRP92075', '0100BRP92076', '0100BRP92077', '0100BRP92078', '0100BRP92079', '0100BRP92080', '0100BRP92081', '0100BRP92082', '0100BRX32920', '0100BRX32921', '0100BRX32922', '0100BRX43052', '0100BRX43055', '0100BRZ00678', '0100BRZ00681', '0100BRZ00686', '0100BRZ00687', '0100BRZ00692', '0100BRZ00694', '0100BRZ00695', '0100BRZ00696', '0100BRZ00698', '0100BRZ00699', '0100BRZ00702', '0100BRZ00703', '0100BRZ00704', '0100BRZ00705', '0100BRZ01655', '0100BRZ01656', '0100BRZ01657', '0100BRZ01658', '0100BRZ01659', '0100BRZ01660', '0100BRZ01661', '0100BRZ01662', '0100BRZ01663', '0100BRZ01664', '0100BRZ01665', '0100BRZ01666', '0100BRZ01667', '0100BRZ01668', '0100BRZ01669', '0100BRZ01670', '0100BRZ01671', '0100BRZ01672', '0100BRZ01673', '0100BRZ01674', '0100BRZ01675', '0100BRZ01676', '0100BRZ01677', '0100BRZ01678', '0100BRZ01679', '0100BRZ01680', '0100BRZ01682', '0100BRZ01683', '0100BRZ01684', '0100BRZ01685', '0100BRZ01686', '0100BRZ01687', '0100BRZ01688', '0100BRZ01689', '0100BRZ01690', '0100BRZ01691', '0100BRZ01692', '0100BRZ01693', '0100BRZ01694', '0100BRZ01695', '0100BRZ01696', '0100BRZ01697', '0100BRZ01699', '0100BRZ01700', '0100BRZ01701', '0100BRZ01707', '0100BRZ01708', '0100BRZ01709', '0100BRZ01710', '0100BRZ01713', '0100FBX18331', '0100FBX18336', '0100FBX18337', '0100FBX18339', '0100FBX18342', '0100SGB20368', '0100SGP90563', '0100SGY38500', '0100SGZ01485', '0170BRP91110', '0170BRP91111', '0190SBX18338', '1', '10000001', '1000053203', '1000053204', '1000053205', '1000053206', '1000053207', '1000053208', '1000053209', '1000053210', '1000053211', '1000053212', '1000053214', '1000053216', '1000053217', '1000053218', '1000053219', '1000053220', '1000053221', '1000053222', '1000053223', '1000053227', '1000053228', '1000053229', '1000053230', '1000053231', '1000053276', '1000053287', '1000053288', '1000053305', '1000053310', '1000053311', '1000053312', '100053233', '100053234', '100053236', '100053239', '100053240', '100053241', '100053247', '100053248', '100053249', '100053250', '100053252', '100053254', '100053255', '100053256', '100053257', '100053258', '100053259', '100053260', '100053261', '100053262', '100053263', '100053264', '100053265', '100053266', '100053267', '100053274', '100053275', '100053277', '100053278', '100053279', '100053280', '100053281', '100053283', '100053291', '100053293', '100053294', '100053295', '100053296', '100053297', '100053298', '100053299', '100053300', '100053301', '100053303', '100053304', '100053306', '100053309', '100053313', '100053315', '100053316', '100053317', '100053318', '100053319', '100053320', '100053321', '100053324', '100053325', '100053328', '100053329', '100053330', '100053331', '100053332', '100053333', '100053334', '100053335', '100053337', '100053338', '100053339', '100053340', '100053343', '100053344', '100053345', '100053346']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored the SQL resultset to be column based (not row based as it was previously).
</commit_message>
<xml_diff>
--- a/examples/bristol bus stops/profile.xlsx
+++ b/examples/bristol bus stops/profile.xlsx
@@ -600,7 +600,11 @@
       <c r="B4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
       <c r="D4" t="n">
         <v>1603</v>
       </c>
@@ -802,7 +806,11 @@
       <c r="B7" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
       <c r="D7" t="n">
         <v>1603</v>
       </c>

</xml_diff>